<commit_message>
fix for assignee not working
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberso/Documents/GitHub/xlsTemplate2Jira/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B7938B-9922-044A-9456-A2BB25506509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EF4DF7-8CC6-7945-B691-28B6DB476BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1080" windowWidth="17520" windowHeight="16440" xr2:uid="{F1D54580-B2A1-4D92-8C41-04CAD953553D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="69">
   <si>
     <t>Country</t>
   </si>
@@ -714,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3067A0C3-667A-4A15-9115-4BB275613752}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="D32" sqref="D32:D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1596,6 +1596,1688 @@
         <v>67</v>
       </c>
       <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="11">
+        <v>3885</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+      <c r="D37" s="11">
+        <v>3996</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="4">
+        <v>3</v>
+      </c>
+      <c r="D38" s="11">
+        <v>4107</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="5">
+        <v>4</v>
+      </c>
+      <c r="D39" s="11">
+        <v>4218</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="4">
+        <v>5</v>
+      </c>
+      <c r="D40" s="11">
+        <v>4329</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="5">
+        <v>6</v>
+      </c>
+      <c r="D41" s="11">
+        <v>4440</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="4">
+        <v>7</v>
+      </c>
+      <c r="D42" s="11">
+        <v>4551</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="5">
+        <v>8</v>
+      </c>
+      <c r="D43" s="11">
+        <v>4662</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="4">
+        <v>9</v>
+      </c>
+      <c r="D44" s="11">
+        <v>4773</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="5">
+        <v>10</v>
+      </c>
+      <c r="D45" s="11">
+        <v>4884</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="4">
+        <v>11</v>
+      </c>
+      <c r="D46" s="11">
+        <v>4995</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="5">
+        <v>12</v>
+      </c>
+      <c r="D47" s="11">
+        <v>5106</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I47" s="12"/>
+    </row>
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="4">
+        <v>13</v>
+      </c>
+      <c r="D48" s="11">
+        <v>5217</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I48" s="12"/>
+    </row>
+    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="5">
+        <v>14</v>
+      </c>
+      <c r="D49" s="11">
+        <v>5328</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I49" s="12"/>
+    </row>
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="4">
+        <v>15</v>
+      </c>
+      <c r="D50" s="11">
+        <v>5439</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50" s="12"/>
+    </row>
+    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="5">
+        <v>16</v>
+      </c>
+      <c r="D51" s="11">
+        <v>5550</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="4">
+        <v>17</v>
+      </c>
+      <c r="D52" s="11">
+        <v>5661</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I52" s="12"/>
+    </row>
+    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="5">
+        <v>18</v>
+      </c>
+      <c r="D53" s="11">
+        <v>5772</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I53" s="12"/>
+    </row>
+    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="4">
+        <v>19</v>
+      </c>
+      <c r="D54" s="11">
+        <v>5883</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I54" s="12"/>
+    </row>
+    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="5">
+        <v>20</v>
+      </c>
+      <c r="D55" s="11">
+        <v>5994</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I55" s="12"/>
+    </row>
+    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="4">
+        <v>21</v>
+      </c>
+      <c r="D56" s="11">
+        <v>6105</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G56" t="s">
+        <v>64</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I56" s="12"/>
+    </row>
+    <row r="57" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="5">
+        <v>22</v>
+      </c>
+      <c r="D57" s="11">
+        <v>6216</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I57" s="12"/>
+    </row>
+    <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="4">
+        <v>23</v>
+      </c>
+      <c r="D58" s="11">
+        <v>6327</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I58" s="12"/>
+    </row>
+    <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="5">
+        <v>24</v>
+      </c>
+      <c r="D59" s="11">
+        <v>6438</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I59" s="12"/>
+    </row>
+    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="4">
+        <v>25</v>
+      </c>
+      <c r="D60" s="11">
+        <v>6549</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I60" s="12"/>
+    </row>
+    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="5">
+        <v>26</v>
+      </c>
+      <c r="D61" s="11">
+        <v>6660</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I61" s="12"/>
+    </row>
+    <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="4">
+        <v>27</v>
+      </c>
+      <c r="D62" s="11">
+        <v>6771</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I62" s="12"/>
+    </row>
+    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="5">
+        <v>28</v>
+      </c>
+      <c r="D63" s="11">
+        <v>6882</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I63" s="12"/>
+    </row>
+    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="4">
+        <v>29</v>
+      </c>
+      <c r="D64" s="11">
+        <v>6993</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I64" s="12"/>
+    </row>
+    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="5">
+        <v>30</v>
+      </c>
+      <c r="D65" s="11">
+        <v>7104</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I65" s="12"/>
+    </row>
+    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="4">
+        <v>31</v>
+      </c>
+      <c r="D66" s="11">
+        <v>7215</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I66" s="12"/>
+    </row>
+    <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" s="5">
+        <v>32</v>
+      </c>
+      <c r="D67" s="11">
+        <v>7326</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I67" s="12"/>
+    </row>
+    <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="4">
+        <v>33</v>
+      </c>
+      <c r="D68" s="11">
+        <v>7437</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G68" t="s">
+        <v>64</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I68" s="12"/>
+    </row>
+    <row r="69" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="5">
+        <v>34</v>
+      </c>
+      <c r="D69" s="11">
+        <v>7548</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G69" t="s">
+        <v>64</v>
+      </c>
+      <c r="H69" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I69" s="12"/>
+    </row>
+    <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1</v>
+      </c>
+      <c r="D70" s="11">
+        <v>7659</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G70" t="s">
+        <v>64</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I70" s="12"/>
+    </row>
+    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="5">
+        <v>2</v>
+      </c>
+      <c r="D71" s="11">
+        <v>7770</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I71" s="12"/>
+    </row>
+    <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="4">
+        <v>3</v>
+      </c>
+      <c r="D72" s="11">
+        <v>7881</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I72" s="12"/>
+    </row>
+    <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" s="5">
+        <v>4</v>
+      </c>
+      <c r="D73" s="11">
+        <v>7992</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G73" t="s">
+        <v>64</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I73" s="12"/>
+    </row>
+    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" s="4">
+        <v>5</v>
+      </c>
+      <c r="D74" s="11">
+        <v>8103</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I74" s="12"/>
+    </row>
+    <row r="75" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="5">
+        <v>6</v>
+      </c>
+      <c r="D75" s="11">
+        <v>8214</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I75" s="12"/>
+    </row>
+    <row r="76" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="4">
+        <v>7</v>
+      </c>
+      <c r="D76" s="11">
+        <v>8325</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I76" s="12"/>
+    </row>
+    <row r="77" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="5">
+        <v>8</v>
+      </c>
+      <c r="D77" s="11">
+        <v>8436</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I77" s="12"/>
+    </row>
+    <row r="78" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="4">
+        <v>9</v>
+      </c>
+      <c r="D78" s="11">
+        <v>8547</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G78" t="s">
+        <v>64</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I78" s="12"/>
+    </row>
+    <row r="79" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" s="5">
+        <v>10</v>
+      </c>
+      <c r="D79" s="11">
+        <v>8658</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I79" s="12"/>
+    </row>
+    <row r="80" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" s="4">
+        <v>11</v>
+      </c>
+      <c r="D80" s="11">
+        <v>8769</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G80" s="7"/>
+      <c r="H80" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I80" s="12"/>
+    </row>
+    <row r="81" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C81" s="5">
+        <v>12</v>
+      </c>
+      <c r="D81" s="11">
+        <v>8880</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G81" t="s">
+        <v>64</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I81" s="12"/>
+    </row>
+    <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" s="4">
+        <v>13</v>
+      </c>
+      <c r="D82" s="11">
+        <v>8991</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I82" s="12"/>
+    </row>
+    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" s="5">
+        <v>14</v>
+      </c>
+      <c r="D83" s="11">
+        <v>9102</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I83" s="12"/>
+    </row>
+    <row r="84" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C84" s="4">
+        <v>15</v>
+      </c>
+      <c r="D84" s="11">
+        <v>9213</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I84" s="12"/>
+    </row>
+    <row r="85" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="5">
+        <v>16</v>
+      </c>
+      <c r="D85" s="11">
+        <v>9324</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I85" s="12"/>
+    </row>
+    <row r="86" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="4">
+        <v>17</v>
+      </c>
+      <c r="D86" s="11">
+        <v>9435</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H86" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I86" s="12"/>
+    </row>
+    <row r="87" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" s="5">
+        <v>18</v>
+      </c>
+      <c r="D87" s="11">
+        <v>9546</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I87" s="12"/>
+    </row>
+    <row r="88" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="4">
+        <v>19</v>
+      </c>
+      <c r="D88" s="11">
+        <v>9657</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H88" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I88" s="12"/>
+    </row>
+    <row r="89" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="5">
+        <v>20</v>
+      </c>
+      <c r="D89" s="11">
+        <v>9768</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I89" s="12"/>
+    </row>
+    <row r="90" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90" s="4">
+        <v>21</v>
+      </c>
+      <c r="D90" s="11">
+        <v>9879</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G90" t="s">
+        <v>64</v>
+      </c>
+      <c r="H90" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I90" s="12"/>
+    </row>
+    <row r="91" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C91" s="5">
+        <v>22</v>
+      </c>
+      <c r="D91" s="11">
+        <v>9990</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G91" t="s">
+        <v>64</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I91" s="12"/>
+    </row>
+    <row r="92" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C92" s="4">
+        <v>23</v>
+      </c>
+      <c r="D92" s="11">
+        <v>10101</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H92" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I92" s="12"/>
+    </row>
+    <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" s="5">
+        <v>24</v>
+      </c>
+      <c r="D93" s="11">
+        <v>10212</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H93" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I93" s="12"/>
+    </row>
+    <row r="94" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="4">
+        <v>25</v>
+      </c>
+      <c r="D94" s="11">
+        <v>10323</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I94" s="12"/>
+    </row>
+    <row r="95" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="5">
+        <v>26</v>
+      </c>
+      <c r="D95" s="11">
+        <v>10434</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I95" s="12"/>
+    </row>
+    <row r="96" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="4">
+        <v>27</v>
+      </c>
+      <c r="D96" s="11">
+        <v>10545</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I96" s="12"/>
+    </row>
+    <row r="97" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" s="5">
+        <v>28</v>
+      </c>
+      <c r="D97" s="11">
+        <v>10656</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I97" s="12"/>
+    </row>
+    <row r="98" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C98" s="4">
+        <v>29</v>
+      </c>
+      <c r="D98" s="11">
+        <v>10767</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H98" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I98" s="12"/>
+    </row>
+    <row r="99" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C99" s="5">
+        <v>30</v>
+      </c>
+      <c r="D99" s="11">
+        <v>10878</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I99" s="12"/>
+    </row>
+    <row r="100" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100" s="4">
+        <v>31</v>
+      </c>
+      <c r="D100" s="11">
+        <v>10989</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H100" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I100" s="12"/>
+    </row>
+    <row r="101" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C101" s="5">
+        <v>32</v>
+      </c>
+      <c r="D101" s="11">
+        <v>11100</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I101" s="12"/>
+    </row>
+    <row r="102" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C102" s="4">
+        <v>33</v>
+      </c>
+      <c r="D102" s="11">
+        <v>11211</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G102" t="s">
+        <v>64</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I102" s="12"/>
+    </row>
+    <row r="103" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C103" s="5">
+        <v>34</v>
+      </c>
+      <c r="D103" s="11">
+        <v>11322</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G103" t="s">
+        <v>64</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I103" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G35" xr:uid="{89C89574-F989-3746-9193-58F8DB006BE1}"/>
@@ -1616,6 +3298,30 @@
     <hyperlink ref="H32" r:id="rId10" xr:uid="{70B87A24-4181-264E-944F-B75621442106}"/>
     <hyperlink ref="H33:H34" r:id="rId11" display="ccc@bogus.net" xr:uid="{87CA7B39-7BE0-7449-B59B-006444A938C1}"/>
     <hyperlink ref="H35" r:id="rId12" xr:uid="{F25537FD-81B6-2741-B494-B1043E6D8616}"/>
+    <hyperlink ref="H36" r:id="rId13" xr:uid="{D64304CD-2BC4-D748-9C89-8233F7069180}"/>
+    <hyperlink ref="H37:H42" r:id="rId14" display="aaa@bogus.net" xr:uid="{0DFD4F28-2D2E-CB42-AD1D-0CA48C65BEA0}"/>
+    <hyperlink ref="H43" r:id="rId15" xr:uid="{17419579-DA1C-8148-8312-251163025480}"/>
+    <hyperlink ref="H44:H49" r:id="rId16" display="bbb@bogus.net" xr:uid="{320FCBC4-1B38-9345-9E21-496FA62222D4}"/>
+    <hyperlink ref="H50" r:id="rId17" xr:uid="{EA351138-4E1F-DF4B-99CE-EDDCF42EFEBB}"/>
+    <hyperlink ref="H51:H56" r:id="rId18" display="ccc@bogus.net" xr:uid="{8A51E75B-A460-334B-96C7-048DBFC2DDF6}"/>
+    <hyperlink ref="H56:H58" r:id="rId19" display="aaa@bogus.net" xr:uid="{B25B0986-0FD1-0046-9F4D-DF2EE5E47AC9}"/>
+    <hyperlink ref="H59" r:id="rId20" xr:uid="{FDB31865-0097-2F46-8171-35BC51DD0C1C}"/>
+    <hyperlink ref="H60:H65" r:id="rId21" display="bbb@bogus.net" xr:uid="{87357369-4C6C-604E-9DB8-91A40AB839D2}"/>
+    <hyperlink ref="H66" r:id="rId22" xr:uid="{8AF46B9A-477C-DE41-A99F-496A8A5BEEFA}"/>
+    <hyperlink ref="H67:H68" r:id="rId23" display="ccc@bogus.net" xr:uid="{46AEE46F-C59B-1D44-BB32-F216FD02D41D}"/>
+    <hyperlink ref="H69" r:id="rId24" xr:uid="{56AAB230-B4AE-3E44-A9E5-0E875DA447A9}"/>
+    <hyperlink ref="H70" r:id="rId25" xr:uid="{54DFA12E-277F-B449-87B3-942E01AAD397}"/>
+    <hyperlink ref="H71:H76" r:id="rId26" display="aaa@bogus.net" xr:uid="{FF9EB9B6-78C5-E049-AD8B-8EB28FCDD40C}"/>
+    <hyperlink ref="H77" r:id="rId27" xr:uid="{A77AF5B9-D515-7C45-976E-12E2D132269A}"/>
+    <hyperlink ref="H78:H83" r:id="rId28" display="bbb@bogus.net" xr:uid="{0AF3DD1C-2899-5D41-A608-C82C2CFD56EC}"/>
+    <hyperlink ref="H84" r:id="rId29" xr:uid="{D8BB0D9F-089B-0A41-92A9-BE793CAEF096}"/>
+    <hyperlink ref="H85:H90" r:id="rId30" display="ccc@bogus.net" xr:uid="{8ED267AE-A512-B743-B95B-6E80AE5E7C79}"/>
+    <hyperlink ref="H90:H92" r:id="rId31" display="aaa@bogus.net" xr:uid="{3CC0225F-7541-2046-9071-74F830B3DE0C}"/>
+    <hyperlink ref="H93" r:id="rId32" xr:uid="{66E31051-C91B-7949-80AF-392102625DC8}"/>
+    <hyperlink ref="H94:H99" r:id="rId33" display="bbb@bogus.net" xr:uid="{DEF55521-F179-2449-B158-B0E602CC9FE5}"/>
+    <hyperlink ref="H100" r:id="rId34" xr:uid="{698807F9-57E9-244F-9469-EDB316092E05}"/>
+    <hyperlink ref="H101:H102" r:id="rId35" display="ccc@bogus.net" xr:uid="{87A03F51-21F2-ED4D-B699-BD224518F4B2}"/>
+    <hyperlink ref="H103" r:id="rId36" xr:uid="{B57C66D3-3DF0-A647-A03B-600CEA03774D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
clean up of code for template processing; made more generic
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberso/Documents/GitHub/xlsTemplate2Jira/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EF4DF7-8CC6-7945-B691-28B6DB476BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1715390B-7EC4-6A47-9A10-91D078571AA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1080" windowWidth="17520" windowHeight="16440" xr2:uid="{F1D54580-B2A1-4D92-8C41-04CAD953553D}"/>
+    <workbookView xWindow="1780" yWindow="1080" windowWidth="16180" windowHeight="15540" xr2:uid="{F1D54580-B2A1-4D92-8C41-04CAD953553D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3067A0C3-667A-4A15-9115-4BB275613752}">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:D103"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3289,39 +3289,39 @@
     <hyperlink ref="H2" r:id="rId1" xr:uid="{87B6A389-E28A-0E40-859F-D027C725A8A7}"/>
     <hyperlink ref="H3:H8" r:id="rId2" display="aaa@bogus.net" xr:uid="{5D239646-2A7B-C841-85EB-6A61C59CD230}"/>
     <hyperlink ref="H9" r:id="rId3" xr:uid="{63521C0D-DCF8-AC42-829F-C400EB3E828D}"/>
-    <hyperlink ref="H10:H15" r:id="rId4" display="bbb@bogus.net" xr:uid="{B966CDFB-A20E-374A-80D4-6852EE7A8C06}"/>
-    <hyperlink ref="H16" r:id="rId5" xr:uid="{F46C3D3C-E704-514A-8B74-39E971598AE8}"/>
-    <hyperlink ref="H17:H22" r:id="rId6" display="ccc@bogus.net" xr:uid="{92968725-68FF-C744-9981-71A86EED2972}"/>
-    <hyperlink ref="H22:H24" r:id="rId7" display="aaa@bogus.net" xr:uid="{A57A7B93-B544-5043-90E5-0B302888AFF7}"/>
-    <hyperlink ref="H25" r:id="rId8" xr:uid="{7D4DBFA1-453F-E64C-B969-A2463357F5E0}"/>
-    <hyperlink ref="H26:H31" r:id="rId9" display="bbb@bogus.net" xr:uid="{1B7ABF2E-1D29-A841-A072-324BFCB700AA}"/>
-    <hyperlink ref="H32" r:id="rId10" xr:uid="{70B87A24-4181-264E-944F-B75621442106}"/>
-    <hyperlink ref="H33:H34" r:id="rId11" display="ccc@bogus.net" xr:uid="{87CA7B39-7BE0-7449-B59B-006444A938C1}"/>
-    <hyperlink ref="H35" r:id="rId12" xr:uid="{F25537FD-81B6-2741-B494-B1043E6D8616}"/>
-    <hyperlink ref="H36" r:id="rId13" xr:uid="{D64304CD-2BC4-D748-9C89-8233F7069180}"/>
-    <hyperlink ref="H37:H42" r:id="rId14" display="aaa@bogus.net" xr:uid="{0DFD4F28-2D2E-CB42-AD1D-0CA48C65BEA0}"/>
-    <hyperlink ref="H43" r:id="rId15" xr:uid="{17419579-DA1C-8148-8312-251163025480}"/>
-    <hyperlink ref="H44:H49" r:id="rId16" display="bbb@bogus.net" xr:uid="{320FCBC4-1B38-9345-9E21-496FA62222D4}"/>
-    <hyperlink ref="H50" r:id="rId17" xr:uid="{EA351138-4E1F-DF4B-99CE-EDDCF42EFEBB}"/>
-    <hyperlink ref="H51:H56" r:id="rId18" display="ccc@bogus.net" xr:uid="{8A51E75B-A460-334B-96C7-048DBFC2DDF6}"/>
-    <hyperlink ref="H56:H58" r:id="rId19" display="aaa@bogus.net" xr:uid="{B25B0986-0FD1-0046-9F4D-DF2EE5E47AC9}"/>
-    <hyperlink ref="H59" r:id="rId20" xr:uid="{FDB31865-0097-2F46-8171-35BC51DD0C1C}"/>
-    <hyperlink ref="H60:H65" r:id="rId21" display="bbb@bogus.net" xr:uid="{87357369-4C6C-604E-9DB8-91A40AB839D2}"/>
-    <hyperlink ref="H66" r:id="rId22" xr:uid="{8AF46B9A-477C-DE41-A99F-496A8A5BEEFA}"/>
-    <hyperlink ref="H67:H68" r:id="rId23" display="ccc@bogus.net" xr:uid="{46AEE46F-C59B-1D44-BB32-F216FD02D41D}"/>
-    <hyperlink ref="H69" r:id="rId24" xr:uid="{56AAB230-B4AE-3E44-A9E5-0E875DA447A9}"/>
-    <hyperlink ref="H70" r:id="rId25" xr:uid="{54DFA12E-277F-B449-87B3-942E01AAD397}"/>
-    <hyperlink ref="H71:H76" r:id="rId26" display="aaa@bogus.net" xr:uid="{FF9EB9B6-78C5-E049-AD8B-8EB28FCDD40C}"/>
-    <hyperlink ref="H77" r:id="rId27" xr:uid="{A77AF5B9-D515-7C45-976E-12E2D132269A}"/>
-    <hyperlink ref="H78:H83" r:id="rId28" display="bbb@bogus.net" xr:uid="{0AF3DD1C-2899-5D41-A608-C82C2CFD56EC}"/>
-    <hyperlink ref="H84" r:id="rId29" xr:uid="{D8BB0D9F-089B-0A41-92A9-BE793CAEF096}"/>
-    <hyperlink ref="H85:H90" r:id="rId30" display="ccc@bogus.net" xr:uid="{8ED267AE-A512-B743-B95B-6E80AE5E7C79}"/>
-    <hyperlink ref="H90:H92" r:id="rId31" display="aaa@bogus.net" xr:uid="{3CC0225F-7541-2046-9071-74F830B3DE0C}"/>
-    <hyperlink ref="H93" r:id="rId32" xr:uid="{66E31051-C91B-7949-80AF-392102625DC8}"/>
-    <hyperlink ref="H94:H99" r:id="rId33" display="bbb@bogus.net" xr:uid="{DEF55521-F179-2449-B158-B0E602CC9FE5}"/>
-    <hyperlink ref="H100" r:id="rId34" xr:uid="{698807F9-57E9-244F-9469-EDB316092E05}"/>
-    <hyperlink ref="H101:H102" r:id="rId35" display="ccc@bogus.net" xr:uid="{87A03F51-21F2-ED4D-B699-BD224518F4B2}"/>
-    <hyperlink ref="H103" r:id="rId36" xr:uid="{B57C66D3-3DF0-A647-A03B-600CEA03774D}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{B966CDFB-A20E-374A-80D4-6852EE7A8C06}"/>
+    <hyperlink ref="H103" r:id="rId5" xr:uid="{B57C66D3-3DF0-A647-A03B-600CEA03774D}"/>
+    <hyperlink ref="H101:H102" r:id="rId6" display="ccc@bogus.net" xr:uid="{87A03F51-21F2-ED4D-B699-BD224518F4B2}"/>
+    <hyperlink ref="H100" r:id="rId7" xr:uid="{698807F9-57E9-244F-9469-EDB316092E05}"/>
+    <hyperlink ref="H94:H99" r:id="rId8" display="bbb@bogus.net" xr:uid="{DEF55521-F179-2449-B158-B0E602CC9FE5}"/>
+    <hyperlink ref="H93" r:id="rId9" xr:uid="{66E31051-C91B-7949-80AF-392102625DC8}"/>
+    <hyperlink ref="H90:H92" r:id="rId10" display="aaa@bogus.net" xr:uid="{3CC0225F-7541-2046-9071-74F830B3DE0C}"/>
+    <hyperlink ref="H85:H90" r:id="rId11" display="ccc@bogus.net" xr:uid="{8ED267AE-A512-B743-B95B-6E80AE5E7C79}"/>
+    <hyperlink ref="H84" r:id="rId12" xr:uid="{D8BB0D9F-089B-0A41-92A9-BE793CAEF096}"/>
+    <hyperlink ref="H78:H83" r:id="rId13" display="bbb@bogus.net" xr:uid="{0AF3DD1C-2899-5D41-A608-C82C2CFD56EC}"/>
+    <hyperlink ref="H77" r:id="rId14" xr:uid="{A77AF5B9-D515-7C45-976E-12E2D132269A}"/>
+    <hyperlink ref="H71:H76" r:id="rId15" display="aaa@bogus.net" xr:uid="{FF9EB9B6-78C5-E049-AD8B-8EB28FCDD40C}"/>
+    <hyperlink ref="H70" r:id="rId16" xr:uid="{54DFA12E-277F-B449-87B3-942E01AAD397}"/>
+    <hyperlink ref="H69" r:id="rId17" xr:uid="{56AAB230-B4AE-3E44-A9E5-0E875DA447A9}"/>
+    <hyperlink ref="H67:H68" r:id="rId18" display="ccc@bogus.net" xr:uid="{46AEE46F-C59B-1D44-BB32-F216FD02D41D}"/>
+    <hyperlink ref="H66" r:id="rId19" xr:uid="{8AF46B9A-477C-DE41-A99F-496A8A5BEEFA}"/>
+    <hyperlink ref="H60:H65" r:id="rId20" display="bbb@bogus.net" xr:uid="{87357369-4C6C-604E-9DB8-91A40AB839D2}"/>
+    <hyperlink ref="H59" r:id="rId21" xr:uid="{FDB31865-0097-2F46-8171-35BC51DD0C1C}"/>
+    <hyperlink ref="H56:H58" r:id="rId22" display="aaa@bogus.net" xr:uid="{B25B0986-0FD1-0046-9F4D-DF2EE5E47AC9}"/>
+    <hyperlink ref="H51:H56" r:id="rId23" display="ccc@bogus.net" xr:uid="{8A51E75B-A460-334B-96C7-048DBFC2DDF6}"/>
+    <hyperlink ref="H50" r:id="rId24" xr:uid="{EA351138-4E1F-DF4B-99CE-EDDCF42EFEBB}"/>
+    <hyperlink ref="H44:H49" r:id="rId25" display="bbb@bogus.net" xr:uid="{320FCBC4-1B38-9345-9E21-496FA62222D4}"/>
+    <hyperlink ref="H43" r:id="rId26" xr:uid="{17419579-DA1C-8148-8312-251163025480}"/>
+    <hyperlink ref="H37:H42" r:id="rId27" display="aaa@bogus.net" xr:uid="{0DFD4F28-2D2E-CB42-AD1D-0CA48C65BEA0}"/>
+    <hyperlink ref="H36" r:id="rId28" xr:uid="{D64304CD-2BC4-D748-9C89-8233F7069180}"/>
+    <hyperlink ref="H35" r:id="rId29" xr:uid="{F25537FD-81B6-2741-B494-B1043E6D8616}"/>
+    <hyperlink ref="H33:H34" r:id="rId30" display="ccc@bogus.net" xr:uid="{87CA7B39-7BE0-7449-B59B-006444A938C1}"/>
+    <hyperlink ref="H32" r:id="rId31" xr:uid="{70B87A24-4181-264E-944F-B75621442106}"/>
+    <hyperlink ref="H26:H31" r:id="rId32" display="bbb@bogus.net" xr:uid="{1B7ABF2E-1D29-A841-A072-324BFCB700AA}"/>
+    <hyperlink ref="H25" r:id="rId33" xr:uid="{7D4DBFA1-453F-E64C-B969-A2463357F5E0}"/>
+    <hyperlink ref="H22:H24" r:id="rId34" display="aaa@bogus.net" xr:uid="{A57A7B93-B544-5043-90E5-0B302888AFF7}"/>
+    <hyperlink ref="H17:H22" r:id="rId35" display="ccc@bogus.net" xr:uid="{92968725-68FF-C744-9981-71A86EED2972}"/>
+    <hyperlink ref="H16" r:id="rId36" xr:uid="{F46C3D3C-E704-514A-8B74-39E971598AE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>